<commit_message>
Bunch of bug fixes and updates to files & documentation
</commit_message>
<xml_diff>
--- a/src/make_cv/files/Awards/personal awards data.xlsx
+++ b/src/make_cv/files/Awards/personal awards data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhelenbr/Codes/make_cv/src/make_cv/files/Awards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3800A6D3-837F-1546-ADE8-DB2A4FFA9EF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51117CED-8F05-CF4A-BE81-6EA25BB87B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17300" activeTab="1" xr2:uid="{E23A13CD-8CAA-9E4B-8575-0E885655E12D}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Title</t>
   </si>
@@ -57,15 +57,6 @@
     <t>School</t>
   </si>
   <si>
-    <t>Million Dollar Club</t>
-  </si>
-  <si>
-    <t>SOE Teaching Excellence</t>
-  </si>
-  <si>
-    <t>Session Chair, ILASS</t>
-  </si>
-  <si>
     <t>Professional</t>
   </si>
   <si>
@@ -73,9 +64,6 @@
   </si>
   <si>
     <t xml:space="preserve">Make an entry in data for every award </t>
-  </si>
-  <si>
-    <t>$\pi\tau\sigma$ Teaching Award</t>
   </si>
   <si>
     <t>Types:</t>
@@ -616,17 +604,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
@@ -651,10 +639,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD645283-76AC-0143-BE6B-3BED9EC12DE1}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -672,59 +660,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>1999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>2007</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>2011</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C17" xr:uid="{F2042D13-CA92-4540-A360-82138B613C4B}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C16">
-      <sortCondition ref="A1:A16"/>
-    </sortState>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C16">
     <sortCondition ref="C2:C16"/>
   </sortState>

</xml_diff>

<commit_message>
Changes to allow control of nrows + changes to get ABET working
</commit_message>
<xml_diff>
--- a/src/make_cv/files/Awards/personal awards data.xlsx
+++ b/src/make_cv/files/Awards/personal awards data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhelenbr/Codes/make_cv/src/make_cv/files/Awards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51117CED-8F05-CF4A-BE81-6EA25BB87B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B618693-7AA6-164B-B3F4-9AAF30E527C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17300" activeTab="1" xr2:uid="{E23A13CD-8CAA-9E4B-8575-0E885655E12D}"/>
   </bookViews>
@@ -592,7 +592,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A10" sqref="A10:A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -642,7 +642,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -668,6 +668,24 @@
     <sortCondition ref="C2:C16"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{760890C1-B29E-8041-9825-968A56E71CD5}">
+      <formula1>1900</formula1>
+      <formula2>2100</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C01A9B06-0654-8F4A-AA03-87FEF758203F}">
+          <x14:formula1>
+            <xm:f>Notes!$A$10:$A$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1:B1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added data validation using openpyxl
</commit_message>
<xml_diff>
--- a/src/make_cv/files/Awards/personal awards data.xlsx
+++ b/src/make_cv/files/Awards/personal awards data.xlsx
@@ -1,104 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bhelenbr/Codes/make_cv/src/make_cv/files/Awards/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B618693-7AA6-164B-B3F4-9AAF30E527C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17300" activeTab="1" xr2:uid="{E23A13CD-8CAA-9E4B-8575-0E885655E12D}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="17300" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Notes" sheetId="3" r:id="rId1"/>
-    <sheet name="Data" sheetId="1" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Notes" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Data!$A$1:$C$17</definedName>
-  </definedNames>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>This sheet is to keep track of awards</t>
-  </si>
-  <si>
-    <t>University</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>School</t>
-  </si>
-  <si>
-    <t>Professional</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Make an entry in data for every award </t>
-  </si>
-  <si>
-    <t>Types:</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -117,12 +61,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -152,75 +96,75 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="1" tint="0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="1" tint="0.499984740745262"/>
       </font>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+          <fgColor theme="0" tint="-0.1499984740745262"/>
+          <bgColor theme="0" tint="-0.1499984740745262"/>
         </patternFill>
       </fill>
       <border>
         <left style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
+          <color theme="0" tint="-0.3499862666707358"/>
         </left>
         <right style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
+          <color theme="0" tint="-0.3499862666707358"/>
         </right>
         <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
+          <color theme="0" tint="-0.3499862666707358"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
+          <color theme="0" tint="-0.3499862666707358"/>
         </bottom>
         <vertical style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
+          <color theme="0" tint="-0.3499862666707358"/>
         </vertical>
         <horizontal style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
+          <color theme="0" tint="-0.3499862666707358"/>
         </horizontal>
       </border>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
+          <fgColor theme="0" tint="-0.1499984740745262"/>
+          <bgColor theme="0" tint="-0.1499984740745262"/>
         </patternFill>
       </fill>
       <border>
         <top style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
+          <color theme="0" tint="-0.3499862666707358"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.34998626667073579"/>
+          <color theme="0" tint="-0.3499862666707358"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
       <fill>
@@ -240,7 +184,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="1"/>
         <color theme="1"/>
       </font>
       <border>
@@ -256,7 +200,7 @@
       <font>
         <color theme="1"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left/>
         <right/>
         <top/>
@@ -267,7 +211,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="PivotStyleLight1 2" table="0" count="11" xr9:uid="{84534529-D9EB-7A4D-9923-32918898A204}">
+    <tableStyle name="PivotStyleLight1 2" table="0" count="11">
       <tableStyleElement type="wholeTable" dxfId="10"/>
       <tableStyleElement type="headerRow" dxfId="9"/>
       <tableStyleElement type="totalRow" dxfId="8"/>
@@ -281,14 +225,74 @@
       <tableStyleElement type="pageFieldValues" dxfId="0"/>
     </tableStyle>
   </tableStyles>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -588,48 +592,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAB97C3C-595B-174A-9C7A-49ACB86D6173}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10:A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>2</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>This sheet is to keep track of awards</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Make an entry in data for every award </t>
+        </is>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>9</v>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Types:</t>
+        </is>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>6</v>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Professional</t>
+        </is>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>5</v>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>School</t>
+        </is>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>3</v>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>University</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -638,54 +660,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD645283-76AC-0143-BE6B-3BED9EC12DE1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="22" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="30.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col width="30.5" customWidth="1" style="2" min="1" max="1"/>
+    <col width="15.6640625" customWidth="1" min="2" max="2"/>
+    <col width="12.6640625" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
+    <row r="1" ht="17" customHeight="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Title</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C16">
-    <sortCondition ref="C2:C16"/>
-  </sortState>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576" xr:uid="{760890C1-B29E-8041-9825-968A56E71CD5}">
+  <dataValidations count="2">
+    <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
+      <formula1>Notes!$A$10:$A$13</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="between">
       <formula1>1900</formula1>
       <formula2>2100</formula2>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C01A9B06-0654-8F4A-AA03-87FEF758203F}">
-          <x14:formula1>
-            <xm:f>Notes!$A$10:$A$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>B1:B1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>